<commit_message>
bw and color versions of figures complete.  updated Package list -pd is now 0.8 for geom_point -substrate revalued to proper names from abbreviations -citation updated -.Rdata for algae and glm updated -updaes to glm and permanova tables for manuscript -export data for table 1
</commit_message>
<xml_diff>
--- a/glm_mod.xlsx
+++ b/glm_mod.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>term</t>
   </si>
@@ -68,12 +68,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>(Intercept)</t>
   </si>
   <si>
@@ -86,22 +80,13 @@
     <t>Sphingobacteria</t>
   </si>
   <si>
-    <t>time</t>
+    <t>k__Fungi_unclassified</t>
   </si>
   <si>
     <t>nh4</t>
   </si>
   <si>
-    <t>k__Fungi_unclassified</t>
-  </si>
-  <si>
-    <t>typebacteria</t>
-  </si>
-  <si>
-    <t>typefungus</t>
-  </si>
-  <si>
-    <t>Oxyphotobacteria</t>
+    <t>Flavobacteria</t>
   </si>
   <si>
     <t>PE and PVC</t>
@@ -187,22 +172,22 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3195</v>
+        <v>0.3255</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03849</v>
+        <v>0.03837</v>
       </c>
       <c r="E2" t="n">
-        <v>8.301</v>
+        <v>8.483</v>
       </c>
       <c r="F2" t="n">
-        <v>2.455E-12</v>
+        <v>9.933E-13</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -210,22 +195,22 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.002962</v>
+        <v>-0.002961</v>
       </c>
       <c r="D3" t="n">
-        <v>1.447E-4</v>
+        <v>1.453E-4</v>
       </c>
       <c r="E3" t="n">
-        <v>-20.46</v>
+        <v>-20.38</v>
       </c>
       <c r="F3" t="n">
-        <v>4.285E-33</v>
+        <v>3.448E-33</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -233,22 +218,22 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>1.337E-4</v>
+        <v>1.328E-4</v>
       </c>
       <c r="D4" t="n">
-        <v>9.375E-6</v>
+        <v>9.393E-6</v>
       </c>
       <c r="E4" t="n">
-        <v>14.26</v>
+        <v>14.14</v>
       </c>
       <c r="F4" t="n">
-        <v>1.995E-23</v>
+        <v>2.3749999999999999E-23</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -256,22 +241,22 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>6.19</v>
+        <v>6.32</v>
       </c>
       <c r="D5" t="n">
-        <v>4.077</v>
+        <v>4.093</v>
       </c>
       <c r="E5" t="n">
-        <v>1.518</v>
+        <v>1.544</v>
       </c>
       <c r="F5" t="n">
-        <v>0.133</v>
+        <v>0.1266</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -279,22 +264,22 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="n">
-        <v>7.315</v>
+        <v>-0.4917</v>
       </c>
       <c r="D6" t="n">
-        <v>1.455</v>
+        <v>0.07174</v>
       </c>
       <c r="E6" t="n">
-        <v>5.027</v>
+        <v>-6.854</v>
       </c>
       <c r="F6" t="n">
-        <v>1.422E-6</v>
+        <v>1.685E-10</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
@@ -302,22 +287,22 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0775</v>
+        <v>-0.001419</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01489</v>
+        <v>2.843E-4</v>
       </c>
       <c r="E7" t="n">
-        <v>-5.205</v>
+        <v>-4.99</v>
       </c>
       <c r="F7" t="n">
-        <v>6.383E-7</v>
+        <v>1.636E-6</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
@@ -325,22 +310,22 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.05787</v>
+        <v>6.905E-5</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01081</v>
+        <v>1.805E-5</v>
       </c>
       <c r="E8" t="n">
-        <v>-5.355</v>
+        <v>3.825</v>
       </c>
       <c r="F8" t="n">
-        <v>3.202E-7</v>
+        <v>1.903E-4</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -348,22 +333,22 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2.054</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.409</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.458</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.147</v>
+      </c>
+      <c r="G9" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2.168</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.392</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1.557</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.1215</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10">
@@ -371,22 +356,22 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1554</v>
+        <v>1.918</v>
       </c>
       <c r="D10" t="n">
-        <v>0.08205</v>
+        <v>0.3307</v>
       </c>
       <c r="E10" t="n">
-        <v>1.894</v>
+        <v>5.801</v>
       </c>
       <c r="F10" t="n">
-        <v>0.05954</v>
+        <v>2.123E-8</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11">
@@ -394,22 +379,22 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-6.687E-5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9.894E-6</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-6.758</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.091E-10</v>
+      </c>
+      <c r="G11" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" t="n">
-        <v>-0.1608</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.07592</v>
-      </c>
-      <c r="E11" t="n">
-        <v>-2.118</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.03522</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -417,22 +402,22 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.04325</v>
+        <v>-0.0126</v>
       </c>
       <c r="D12" t="n">
-        <v>0.09837</v>
+        <v>0.002279</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.4397</v>
+        <v>-5.53</v>
       </c>
       <c r="F12" t="n">
-        <v>0.6606</v>
+        <v>8.504E-8</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
@@ -443,65 +428,19 @@
         <v>24</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01236</v>
+        <v>-33.97</v>
       </c>
       <c r="D13" t="n">
-        <v>0.002852</v>
+        <v>21.79</v>
       </c>
       <c r="E13" t="n">
-        <v>4.333</v>
+        <v>-1.559</v>
       </c>
       <c r="F13" t="n">
-        <v>2.202E-5</v>
+        <v>0.1204</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="n">
-        <v>-8.981E-4</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1.365E-4</v>
-      </c>
-      <c r="E14" t="n">
-        <v>-6.578</v>
-      </c>
-      <c r="F14" t="n">
-        <v>3.233E-10</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="n">
-        <v>-1.966</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1.059</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-1.856</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.06478</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
glm mods are stable
</commit_message>
<xml_diff>
--- a/glm_mod.xlsx
+++ b/glm_mod.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>term</t>
   </si>
@@ -71,19 +71,22 @@
     <t>(Intercept)</t>
   </si>
   <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>nh4</t>
+  </si>
+  <si>
+    <t>Sphingobacteria</t>
+  </si>
+  <si>
     <t>srp</t>
   </si>
   <si>
     <t>no3</t>
   </si>
   <si>
-    <t>Sphingobacteria</t>
-  </si>
-  <si>
     <t>k__Fungi_unclassified</t>
-  </si>
-  <si>
-    <t>nh4</t>
   </si>
   <si>
     <t>Flavobacteria</t>
@@ -175,19 +178,19 @@
         <v>18</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3255</v>
+        <v>19.65</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03837</v>
+        <v>0.738</v>
       </c>
       <c r="E2" t="n">
-        <v>8.483</v>
+        <v>26.63</v>
       </c>
       <c r="F2" t="n">
-        <v>9.933E-13</v>
+        <v>3.29E-41</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
@@ -198,19 +201,19 @@
         <v>19</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.002961</v>
+        <v>-0.1957</v>
       </c>
       <c r="D3" t="n">
-        <v>1.453E-4</v>
+        <v>0.007594</v>
       </c>
       <c r="E3" t="n">
-        <v>-20.38</v>
+        <v>-25.76</v>
       </c>
       <c r="F3" t="n">
-        <v>3.448E-33</v>
+        <v>3.401E-40</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -221,19 +224,19 @@
         <v>20</v>
       </c>
       <c r="C4" t="n">
-        <v>1.328E-4</v>
+        <v>-0.1438</v>
       </c>
       <c r="D4" t="n">
-        <v>9.393E-6</v>
+        <v>0.005487</v>
       </c>
       <c r="E4" t="n">
-        <v>14.14</v>
+        <v>-26.21</v>
       </c>
       <c r="F4" t="n">
-        <v>2.3749999999999999E-23</v>
+        <v>1.012E-40</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
@@ -256,7 +259,7 @@
         <v>0.1266</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -279,7 +282,7 @@
         <v>1.685E-10</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -287,7 +290,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C7" t="n">
         <v>-0.001419</v>
@@ -302,7 +305,7 @@
         <v>1.636E-6</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
@@ -310,7 +313,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C8" t="n">
         <v>6.905E-5</v>
@@ -325,7 +328,7 @@
         <v>1.903E-4</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
@@ -333,7 +336,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" t="n">
         <v>2.054</v>
@@ -348,7 +351,7 @@
         <v>0.147</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
@@ -359,19 +362,19 @@
         <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>1.918</v>
+        <v>13.07</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3307</v>
+        <v>1.925</v>
       </c>
       <c r="E10" t="n">
-        <v>5.801</v>
+        <v>6.789</v>
       </c>
       <c r="F10" t="n">
-        <v>2.123E-8</v>
+        <v>9.129E-11</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -379,13 +382,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="n">
-        <v>-6.687E-5</v>
+        <v>-0.1333</v>
       </c>
       <c r="D11" t="n">
-        <v>9.894E-6</v>
+        <v>0.01973</v>
       </c>
       <c r="E11" t="n">
         <v>-6.758</v>
@@ -394,7 +397,7 @@
         <v>1.091E-10</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
@@ -402,22 +405,22 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.0126</v>
+        <v>-0.09854</v>
       </c>
       <c r="D12" t="n">
-        <v>0.002279</v>
+        <v>0.01431</v>
       </c>
       <c r="E12" t="n">
-        <v>-5.53</v>
+        <v>-6.887</v>
       </c>
       <c r="F12" t="n">
-        <v>8.504E-8</v>
+        <v>5.172E-11</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
@@ -425,7 +428,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="n">
         <v>-33.97</v>
@@ -440,7 +443,7 @@
         <v>0.1204</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>